<commit_message>
Modificado backlog para sprint 2 Adicionado arquico com lembretes para a sprint 1
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Product BackLog.xlsx
+++ b/Trunk/Doc/Product BackLog.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23812"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t>#</t>
   </si>
@@ -160,13 +163,28 @@
   </si>
   <si>
     <t>Sprint</t>
+  </si>
+  <si>
+    <t>Porcentagem</t>
+  </si>
+  <si>
+    <t>Obs.</t>
+  </si>
+  <si>
+    <t>Falta interface</t>
+  </si>
+  <si>
+    <t>Mudar chamada do webservice</t>
+  </si>
+  <si>
+    <t>Falta validação e chamada do webservice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,8 +200,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,8 +236,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -216,42 +256,52 @@
         <color theme="0"/>
       </left>
       <right/>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color theme="0"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -272,19 +322,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:H47" totalsRowShown="0">
-  <autoFilter ref="B3:H47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:J47" totalsRowShown="0">
+  <autoFilter ref="B3:J47">
     <filterColumn colId="2">
       <filters>
         <filter val="Web"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="6"/>
   </autoFilter>
   <sortState ref="B4:G48">
     <sortCondition descending="1" ref="G3:G49"/>
   </sortState>
-  <tableColumns count="7">
+  <tableColumns count="9">
     <tableColumn id="1" name="#"/>
     <tableColumn id="2" name="User History"/>
     <tableColumn id="3" name="Plataform"/>
@@ -294,6 +343,8 @@
       <calculatedColumnFormula>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Sprint"/>
+    <tableColumn id="7" name="Porcentagem"/>
+    <tableColumn id="9" name="Obs."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -554,44 +605,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" activeCellId="1" sqref="E5:E20 E24"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="3" max="3" width="101.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="1.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
+    <col min="3" max="3" width="101.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="10" max="10" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="6.75" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:8" ht="19.5" thickBot="1">
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="2:8">
+    <row r="1" spans="2:10" ht="6.75" customHeight="1"/>
+    <row r="2" spans="2:10" ht="18">
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="2:10">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -613,8 +668,14 @@
       <c r="H3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" hidden="1">
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" hidden="1">
       <c r="B4">
         <v>3</v>
       </c>
@@ -635,7 +696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:10">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -658,8 +719,14 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:8">
+      <c r="I5">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -682,8 +749,14 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:8">
+      <c r="I6">
+        <v>80</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
       <c r="B7" s="3">
         <v>33</v>
       </c>
@@ -706,8 +779,14 @@
       <c r="H7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" hidden="1">
+      <c r="I7">
+        <v>80</v>
+      </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" hidden="1">
       <c r="B8">
         <v>6</v>
       </c>
@@ -728,7 +807,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="9" spans="2:8" hidden="1">
+    <row r="9" spans="2:10" hidden="1">
       <c r="B9">
         <v>9</v>
       </c>
@@ -749,7 +828,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:10">
       <c r="B10" s="3">
         <v>19</v>
       </c>
@@ -772,8 +851,14 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:8">
+      <c r="I10">
+        <v>80</v>
+      </c>
+      <c r="J10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
       <c r="B11" s="3">
         <v>22</v>
       </c>
@@ -796,8 +881,14 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="I11">
+        <v>80</v>
+      </c>
+      <c r="J11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
       <c r="B12" s="3">
         <v>26</v>
       </c>
@@ -820,8 +911,14 @@
       <c r="H12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" hidden="1">
+      <c r="I12">
+        <v>80</v>
+      </c>
+      <c r="J12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" hidden="1">
       <c r="B13">
         <v>34</v>
       </c>
@@ -842,7 +939,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:10">
       <c r="B14" s="3">
         <v>35</v>
       </c>
@@ -865,8 +962,14 @@
       <c r="H14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" hidden="1">
+      <c r="I14">
+        <v>80</v>
+      </c>
+      <c r="J14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" hidden="1">
       <c r="B15">
         <v>2</v>
       </c>
@@ -887,7 +990,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:10">
       <c r="B16" s="3">
         <v>21</v>
       </c>
@@ -910,8 +1013,14 @@
       <c r="H16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="I16">
+        <v>80</v>
+      </c>
+      <c r="J16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
       <c r="B17" s="3">
         <v>27</v>
       </c>
@@ -934,8 +1043,14 @@
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" hidden="1">
+      <c r="I17">
+        <v>80</v>
+      </c>
+      <c r="J17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" hidden="1">
       <c r="B18">
         <v>23</v>
       </c>
@@ -956,7 +1071,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:10">
       <c r="B19" s="3">
         <v>24</v>
       </c>
@@ -979,8 +1094,14 @@
       <c r="H19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="I19">
+        <v>80</v>
+      </c>
+      <c r="J19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
       <c r="B20" s="3">
         <v>29</v>
       </c>
@@ -1003,8 +1124,14 @@
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" hidden="1">
+      <c r="I20">
+        <v>80</v>
+      </c>
+      <c r="J20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" hidden="1">
       <c r="B21">
         <v>11</v>
       </c>
@@ -1025,7 +1152,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="22" spans="2:8" hidden="1">
+    <row r="22" spans="2:10" hidden="1">
       <c r="B22">
         <v>16</v>
       </c>
@@ -1046,11 +1173,11 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
-      <c r="B23">
+    <row r="23" spans="2:10">
+      <c r="B23" s="4">
         <v>17</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
@@ -1066,8 +1193,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
+      <c r="H23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
       <c r="B24" s="3">
         <v>25</v>
       </c>
@@ -1090,8 +1220,14 @@
       <c r="H24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" hidden="1">
+      <c r="I24">
+        <v>80</v>
+      </c>
+      <c r="J24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" hidden="1">
       <c r="B25">
         <v>37</v>
       </c>
@@ -1112,7 +1248,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="2:8" hidden="1">
+    <row r="26" spans="2:10" hidden="1">
       <c r="B26">
         <v>38</v>
       </c>
@@ -1133,11 +1269,11 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
-      <c r="B27">
+    <row r="27" spans="2:10">
+      <c r="B27" s="4">
         <v>39</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D27" t="s">
@@ -1153,8 +1289,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" hidden="1">
+      <c r="H27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" hidden="1">
       <c r="B28">
         <v>40</v>
       </c>
@@ -1175,11 +1314,11 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
-      <c r="B29">
+    <row r="29" spans="2:10">
+      <c r="B29" s="4">
         <v>41</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="4" t="s">
         <v>37</v>
       </c>
       <c r="D29" t="s">
@@ -1195,8 +1334,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" hidden="1">
+      <c r="H29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" hidden="1">
       <c r="B30">
         <v>42</v>
       </c>
@@ -1217,11 +1359,11 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
-      <c r="B31">
+    <row r="31" spans="2:10">
+      <c r="B31" s="4">
         <v>43</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D31" t="s">
@@ -1237,8 +1379,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1.6</v>
       </c>
-    </row>
-    <row r="32" spans="2:8">
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
       <c r="B32">
         <v>10</v>
       </c>
@@ -1259,7 +1404,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:8">
       <c r="B33">
         <v>28</v>
       </c>
@@ -1280,7 +1425,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:8">
       <c r="B34">
         <v>7</v>
       </c>
@@ -1301,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:8">
       <c r="B35">
         <v>8</v>
       </c>
@@ -1322,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:7" hidden="1">
+    <row r="36" spans="2:8" hidden="1">
       <c r="B36">
         <v>13</v>
       </c>
@@ -1343,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:8">
       <c r="B37">
         <v>14</v>
       </c>
@@ -1364,11 +1509,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
-      <c r="B38">
+    <row r="38" spans="2:8">
+      <c r="B38" s="4">
         <v>18</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D38" t="s">
@@ -1384,12 +1529,15 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="2:7">
-      <c r="B39">
+      <c r="H38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="4">
         <v>20</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D39" t="s">
@@ -1405,12 +1553,15 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="2:7">
-      <c r="B40">
+      <c r="H39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="4">
         <v>30</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D40" t="s">
@@ -1426,8 +1577,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="2:7">
+      <c r="H40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
       <c r="B41">
         <v>32</v>
       </c>
@@ -1448,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:7" hidden="1">
+    <row r="42" spans="2:8" hidden="1">
       <c r="B42">
         <v>44</v>
       </c>
@@ -1469,7 +1623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:7">
+    <row r="43" spans="2:8">
       <c r="B43">
         <v>45</v>
       </c>
@@ -1490,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:7" hidden="1">
+    <row r="44" spans="2:8" hidden="1">
       <c r="B44">
         <v>46</v>
       </c>
@@ -1511,11 +1665,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:7">
-      <c r="B45">
+    <row r="45" spans="2:8">
+      <c r="B45" s="4">
         <v>31</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D45" t="s">
@@ -1531,8 +1685,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" hidden="1">
+      <c r="H45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" hidden="1">
       <c r="B46">
         <v>15</v>
       </c>
@@ -1553,15 +1710,20 @@
         <v>0.61904761904761907</v>
       </c>
     </row>
-    <row r="47" spans="2:7" hidden="1"/>
+    <row r="47" spans="2:8" hidden="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização para adequar a funcionalidade da Entidade Rota
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Product BackLog.xlsx
+++ b/Trunk/Doc/Product BackLog.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\Unibratec\Repositorios\fusioness\Trunk\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="-435" windowWidth="25605" windowHeight="16005"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -328,6 +333,11 @@
       <filters>
         <filter val="Web"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <sortState ref="B4:G48">
@@ -605,7 +615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,27 +623,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="3" max="3" width="101.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" customWidth="1"/>
-    <col min="10" max="10" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="6.75" customHeight="1"/>
-    <row r="2" spans="2:10" ht="18">
+    <row r="1" spans="2:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
@@ -646,7 +655,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -675,7 +684,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="2:10" hidden="1">
+    <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -696,7 +705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -726,7 +735,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -756,7 +765,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>33</v>
       </c>
@@ -786,7 +795,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="2:10" hidden="1">
+    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>6</v>
       </c>
@@ -807,7 +816,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="9" spans="2:10" hidden="1">
+    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>9</v>
       </c>
@@ -828,7 +837,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>19</v>
       </c>
@@ -858,7 +867,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>22</v>
       </c>
@@ -888,7 +897,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>26</v>
       </c>
@@ -918,7 +927,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:10" hidden="1">
+    <row r="13" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>34</v>
       </c>
@@ -939,7 +948,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>35</v>
       </c>
@@ -969,7 +978,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="2:10" hidden="1">
+    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2</v>
       </c>
@@ -990,7 +999,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="16" spans="2:10">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>21</v>
       </c>
@@ -1020,7 +1029,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>27</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:10" hidden="1">
+    <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>23</v>
       </c>
@@ -1071,7 +1080,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>24</v>
       </c>
@@ -1101,7 +1110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>29</v>
       </c>
@@ -1131,7 +1140,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:10" hidden="1">
+    <row r="21" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>11</v>
       </c>
@@ -1152,7 +1161,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="22" spans="2:10" hidden="1">
+    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>16</v>
       </c>
@@ -1173,7 +1182,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="23" spans="2:10">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>17</v>
       </c>
@@ -1197,7 +1206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <v>25</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:10" hidden="1">
+    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>37</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="2:10" hidden="1">
+    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>38</v>
       </c>
@@ -1269,7 +1278,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="27" spans="2:10">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>39</v>
       </c>
@@ -1293,7 +1302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:10" hidden="1">
+    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>40</v>
       </c>
@@ -1314,7 +1323,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="29" spans="2:10">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>41</v>
       </c>
@@ -1338,7 +1347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:10" hidden="1">
+    <row r="30" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>42</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="31" spans="2:10">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>43</v>
       </c>
@@ -1383,7 +1392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:10">
+    <row r="32" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>10</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>28</v>
       </c>
@@ -1425,7 +1434,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>7</v>
       </c>
@@ -1446,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>8</v>
       </c>
@@ -1467,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:8" hidden="1">
+    <row r="36" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>13</v>
       </c>
@@ -1488,7 +1497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>14</v>
       </c>
@@ -1509,7 +1518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>18</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>20</v>
       </c>
@@ -1557,7 +1566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
         <v>30</v>
       </c>
@@ -1581,7 +1590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>32</v>
       </c>
@@ -1602,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:8" hidden="1">
+    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>44</v>
       </c>
@@ -1623,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>45</v>
       </c>
@@ -1644,7 +1653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:8" hidden="1">
+    <row r="44" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>46</v>
       </c>
@@ -1665,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>31</v>
       </c>
@@ -1689,7 +1698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="2:8" hidden="1">
+    <row r="46" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>15</v>
       </c>
@@ -1710,7 +1719,7 @@
         <v>0.61904761904761907</v>
       </c>
     </row>
-    <row r="47" spans="2:8" hidden="1"/>
+    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:J2"/>

</xml_diff>

<commit_message>
Add US sprint #4
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Product BackLog.xlsx
+++ b/Trunk/Doc/Product BackLog.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto Final\fusioness\Trunk\Doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-435" windowWidth="25605" windowHeight="16005"/>
+    <workbookView xWindow="0" yWindow="-435" windowWidth="20640" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>#</t>
   </si>
@@ -177,9 +172,6 @@
   </si>
   <si>
     <t>Mudar chamada do webservice</t>
-  </si>
-  <si>
-    <t>Falta validação e chamada do webservice</t>
   </si>
   <si>
     <t xml:space="preserve">Como usuário gostaria de fazer Login </t>
@@ -189,7 +181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,8 +213,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +250,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,7 +297,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -304,24 +310,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -343,9 +351,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:J47" totalsRowShown="0">
-  <autoFilter ref="B3:J47"/>
-  <sortState ref="B4:J46">
-    <sortCondition ref="B3:B46"/>
+  <autoFilter ref="B3:J47">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="4"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState ref="B5:J46">
+    <sortCondition ref="H3:H47"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="#"/>
@@ -619,7 +633,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J47"/>
+  <dimension ref="B1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +702,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -709,7 +723,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -739,7 +753,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -769,7 +783,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -790,52 +804,67 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
+    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G8">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="H8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>80</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G9">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>80</v>
+      </c>
+      <c r="J9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
@@ -856,28 +885,37 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
+    <row r="11" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G11">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>80</v>
+      </c>
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>11</v>
       </c>
@@ -898,7 +936,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>13</v>
       </c>
@@ -919,28 +957,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
+    <row r="14" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14">
         <v>5</v>
       </c>
       <c r="G14">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>80</v>
+      </c>
+      <c r="J14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>15</v>
       </c>
@@ -961,7 +1008,7 @@
         <v>0.61904761904761907</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>16</v>
       </c>
@@ -982,12 +1029,12 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
-        <v>17</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>21</v>
+    <row r="17" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>25</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -1003,93 +1050,102 @@
         <v>1.6</v>
       </c>
       <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="4">
-        <v>18</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-      <c r="G18">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
-        <v>19</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
       <c r="F19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G19">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.6666666666666665</v>
+        <v>2.5</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3">
+        <v>29</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>80</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="4">
-        <v>20</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
-      </c>
-      <c r="G20">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
@@ -1098,28 +1154,25 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G21">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <v>1</v>
       </c>
       <c r="I21">
-        <v>80</v>
-      </c>
-      <c r="J21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -1144,7 +1197,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>23</v>
       </c>
@@ -1165,277 +1218,247 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="3">
-        <v>24</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>25</v>
+    <row r="24" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>17</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G24">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6666666666666667</v>
+        <v>1.6</v>
       </c>
       <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24">
-        <v>80</v>
-      </c>
-      <c r="J24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="3">
-        <v>25</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>18</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G25">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>20</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>30</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>31</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>39</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1.6</v>
       </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-      <c r="I25">
-        <v>80</v>
-      </c>
-      <c r="J25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
-        <v>26</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26">
-        <v>3</v>
-      </c>
-      <c r="F26">
-        <v>8</v>
-      </c>
-      <c r="G26">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.6666666666666665</v>
-      </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
-      <c r="I26">
-        <v>80</v>
-      </c>
-      <c r="J26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="3">
-        <v>27</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27">
+      <c r="H29">
         <v>2</v>
       </c>
-      <c r="F27">
-        <v>5</v>
-      </c>
-      <c r="G27">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.5</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>80</v>
-      </c>
-      <c r="J27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>28</v>
-      </c>
-      <c r="C28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-      <c r="G28">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="3">
-        <v>29</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29">
-        <v>3</v>
-      </c>
-      <c r="F29">
-        <v>5</v>
-      </c>
-      <c r="G29">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>80</v>
-      </c>
-      <c r="J29" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F30">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G30">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="H30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G31">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>0.66666666666666663</v>
+        <v>1.6</v>
       </c>
       <c r="H31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>32</v>
-      </c>
-      <c r="C32" t="s">
-        <v>32</v>
+        <v>7</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
       <c r="E32">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G32">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="3">
-        <v>33</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>41</v>
+      <c r="H32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="8">
+        <v>8</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F33">
         <v>8</v>
       </c>
       <c r="G33">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H33">
         <v>4</v>
       </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>80</v>
-      </c>
-      <c r="J33" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>34</v>
       </c>
@@ -1456,114 +1479,108 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="3">
-        <v>35</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>33</v>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="8">
+        <v>10</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
       </c>
       <c r="E35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F35">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G35">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.6666666666666665</v>
+        <v>1.5</v>
       </c>
       <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <v>80</v>
-      </c>
-      <c r="J35" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="8">
+        <v>14</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="8">
+        <v>28</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.5</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="8">
+        <v>32</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B39">
         <v>37</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D36" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36">
-        <v>5</v>
-      </c>
-      <c r="F36">
-        <v>8</v>
-      </c>
-      <c r="G36">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>38</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37">
-        <v>5</v>
-      </c>
-      <c r="F37">
-        <v>8</v>
-      </c>
-      <c r="G37">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="4">
-        <v>39</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38">
-        <v>5</v>
-      </c>
-      <c r="F38">
-        <v>8</v>
-      </c>
-      <c r="G38">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>40</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
@@ -1582,36 +1599,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="4">
-        <v>41</v>
-      </c>
-      <c r="C40" s="4" t="s">
+    <row r="40" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.6</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="D40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40">
-        <v>5</v>
-      </c>
-      <c r="F40">
-        <v>8</v>
-      </c>
-      <c r="G40">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>42</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -1630,15 +1647,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="4">
-        <v>43</v>
-      </c>
-      <c r="C42" s="4" t="s">
+    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>42</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42">
         <v>5</v>
@@ -1651,10 +1668,10 @@
         <v>1.6</v>
       </c>
       <c r="H42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>44</v>
       </c>
@@ -1675,11 +1692,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="8">
         <v>45</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
@@ -1695,8 +1712,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>46</v>
       </c>
@@ -1717,12 +1737,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="8">
         <v>47</v>
       </c>
-      <c r="C46" t="s">
-        <v>51</v>
+      <c r="C46" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
@@ -1737,13 +1757,16 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -1758,15 +1781,18 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>0.625</v>
       </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Add Relatorio de Status_sprint_#3_21_10.doc Mudança do Product BackLog.xlsx para refletir o status atual.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Product BackLog.xlsx
+++ b/Trunk/Doc/Product BackLog.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-435" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
   <si>
     <t>#</t>
   </si>
@@ -168,13 +168,28 @@
     <t>Obs.</t>
   </si>
   <si>
-    <t>Falta interface</t>
-  </si>
-  <si>
-    <t>Mudar chamada do webservice</t>
-  </si>
-  <si>
     <t xml:space="preserve">Como usuário gostaria de fazer Login </t>
+  </si>
+  <si>
+    <t>negociar requisito com professor</t>
+  </si>
+  <si>
+    <t>web service pronto</t>
+  </si>
+  <si>
+    <t>so um bool no banco</t>
+  </si>
+  <si>
+    <t>faltam duas msgs de erro para o usuario. Login unico e e-mail unico</t>
+  </si>
+  <si>
+    <t>falta visual</t>
+  </si>
+  <si>
+    <t>Não informado</t>
+  </si>
+  <si>
+    <t>Não iniciado</t>
   </si>
 </sst>
 </file>
@@ -278,8 +293,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -304,32 +329,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+  <cellStyles count="27">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -353,9 +388,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:J47" totalsRowShown="0">
   <autoFilter ref="B3:J47">
     <filterColumn colId="6">
-      <filters>
-        <filter val="4"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <sortState ref="B5:J46">
@@ -641,39 +676,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:J50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" customWidth="1"/>
-    <col min="3" max="3" width="101.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" customWidth="1"/>
+    <col min="3" max="3" width="101.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" customWidth="1"/>
+    <col min="10" max="10" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="6.75" customHeight="1"/>
+    <row r="2" spans="2:10" ht="18">
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="2:10">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -702,7 +738,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" hidden="1">
       <c r="B4">
         <v>3</v>
       </c>
@@ -723,7 +759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -747,13 +783,13 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -777,13 +813,13 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" hidden="1">
       <c r="B7">
         <v>6</v>
       </c>
@@ -804,7 +840,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" s="3">
         <v>19</v>
       </c>
@@ -828,13 +864,13 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
       <c r="B9" s="3">
         <v>21</v>
       </c>
@@ -858,13 +894,13 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" hidden="1">
       <c r="B10">
         <v>9</v>
       </c>
@@ -885,7 +921,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="B11" s="3">
         <v>22</v>
       </c>
@@ -909,13 +945,10 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>80</v>
-      </c>
-      <c r="J11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" hidden="1">
       <c r="B12">
         <v>11</v>
       </c>
@@ -936,7 +969,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="13" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" hidden="1">
       <c r="B13">
         <v>13</v>
       </c>
@@ -957,7 +990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10">
       <c r="B14" s="3">
         <v>24</v>
       </c>
@@ -981,13 +1014,10 @@
         <v>1</v>
       </c>
       <c r="I14">
-        <v>80</v>
-      </c>
-      <c r="J14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" hidden="1">
       <c r="B15">
         <v>15</v>
       </c>
@@ -1008,7 +1038,7 @@
         <v>0.61904761904761907</v>
       </c>
     </row>
-    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" hidden="1">
       <c r="B16">
         <v>16</v>
       </c>
@@ -1029,7 +1059,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="17" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="B17" s="3">
         <v>25</v>
       </c>
@@ -1053,10 +1083,13 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="J17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
       <c r="B18" s="3">
         <v>26</v>
       </c>
@@ -1083,7 +1116,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10">
       <c r="B19" s="3">
         <v>27</v>
       </c>
@@ -1110,7 +1143,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10">
       <c r="B20" s="3">
         <v>29</v>
       </c>
@@ -1134,13 +1167,10 @@
         <v>1</v>
       </c>
       <c r="I20">
-        <v>80</v>
-      </c>
-      <c r="J20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
       <c r="B21" s="3">
         <v>33</v>
       </c>
@@ -1167,7 +1197,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10">
       <c r="B22" s="3">
         <v>35</v>
       </c>
@@ -1191,13 +1221,13 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" hidden="1">
       <c r="B23">
         <v>23</v>
       </c>
@@ -1218,7 +1248,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="24" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10">
       <c r="B24" s="4">
         <v>17</v>
       </c>
@@ -1241,8 +1271,11 @@
       <c r="H24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
       <c r="B25" s="4">
         <v>18</v>
       </c>
@@ -1265,8 +1298,11 @@
       <c r="H25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
       <c r="B26" s="4">
         <v>20</v>
       </c>
@@ -1289,8 +1325,11 @@
       <c r="H26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
       <c r="B27" s="4">
         <v>30</v>
       </c>
@@ -1313,8 +1352,14 @@
       <c r="H27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>50</v>
+      </c>
+      <c r="J27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
       <c r="B28" s="4">
         <v>31</v>
       </c>
@@ -1337,8 +1382,14 @@
       <c r="H28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>50</v>
+      </c>
+      <c r="J28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
       <c r="B29" s="4">
         <v>39</v>
       </c>
@@ -1361,8 +1412,11 @@
       <c r="H29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
       <c r="B30" s="4">
         <v>41</v>
       </c>
@@ -1385,8 +1439,11 @@
       <c r="H30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
       <c r="B31" s="4">
         <v>43</v>
       </c>
@@ -1409,8 +1466,11 @@
       <c r="H31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
       <c r="B32">
         <v>7</v>
       </c>
@@ -1433,32 +1493,41 @@
       <c r="H32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="8">
-        <v>8</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>12</v>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33">
+        <v>37</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F33">
         <v>8</v>
       </c>
       <c r="G33">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="H33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" hidden="1">
       <c r="B34">
         <v>34</v>
       </c>
@@ -1479,93 +1548,102 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="8">
-        <v>10</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>14</v>
+    <row r="35" spans="2:10">
+      <c r="B35">
+        <v>38</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F35">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G35">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="H35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="8">
-        <v>14</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="I35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36">
+        <v>40</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36">
         <v>5</v>
       </c>
       <c r="F36">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G36">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="H36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="8">
-        <v>28</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>28</v>
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37">
+        <v>42</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F37">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G37">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="H37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="8">
-        <v>32</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>32</v>
+        <v>3</v>
+      </c>
+      <c r="J37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="6">
+        <v>8</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D38" t="s">
         <v>10</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F38">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G38">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
@@ -1574,104 +1652,119 @@
       <c r="H38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B39">
-        <v>37</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>34</v>
+      <c r="J38" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="6">
+        <v>10</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E39">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F39">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G39">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="H39">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>38</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>35</v>
+        <v>4</v>
+      </c>
+      <c r="J39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="6">
+        <v>14</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E40">
         <v>5</v>
       </c>
       <c r="F40">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G40">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="H40">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>40</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>36</v>
+        <v>4</v>
+      </c>
+      <c r="J40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="6">
+        <v>28</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F41">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G41">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="H41">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>42</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="J41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="6">
+        <v>32</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F42">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G42">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="H42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="J42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" hidden="1">
       <c r="B43">
         <v>44</v>
       </c>
@@ -1692,11 +1785,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="8">
+    <row r="44" spans="2:10">
+      <c r="B44" s="6">
         <v>45</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
@@ -1715,8 +1808,11 @@
       <c r="H44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" hidden="1">
       <c r="B45">
         <v>46</v>
       </c>
@@ -1737,12 +1833,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="8">
+    <row r="46" spans="2:10">
+      <c r="B46" s="6">
         <v>47</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>50</v>
+      <c r="C46" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="D46" t="s">
         <v>10</v>
@@ -1760,13 +1856,16 @@
       <c r="H46">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" hidden="1">
       <c r="B47">
         <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D47" t="s">
         <v>9</v>
@@ -1782,17 +1881,17 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="9"/>
+    <row r="50" spans="3:3">
+      <c r="C50" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Add relatorio de status sprint 4 28/10/2013 Renomear Relatorio de Status_sprint_#3_21_10.doc que pertence a Sprint 4 Atualizar Sprint-Backlog-Sprint-04#.xlsx
TODO:
Finalizar o Sprint-Backlog-Sprint-04#.xlsx inserindo as informações faltantes.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Product BackLog.xlsx
+++ b/Trunk/Doc/Product BackLog.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="57">
   <si>
     <t>#</t>
   </si>
@@ -171,18 +171,12 @@
     <t xml:space="preserve">Como usuário gostaria de fazer Login </t>
   </si>
   <si>
-    <t>negociar requisito com professor</t>
-  </si>
-  <si>
     <t>web service pronto</t>
   </si>
   <si>
     <t>so um bool no banco</t>
   </si>
   <si>
-    <t>faltam duas msgs de erro para o usuario. Login unico e e-mail unico</t>
-  </si>
-  <si>
     <t>falta visual</t>
   </si>
   <si>
@@ -190,6 +184,15 @@
   </si>
   <si>
     <t>Não iniciado</t>
+  </si>
+  <si>
+    <t>visual a ser revisado</t>
+  </si>
+  <si>
+    <t>resolver problema de mapeamento</t>
+  </si>
+  <si>
+    <t>falta upload da foto da bicicleta</t>
   </si>
 </sst>
 </file>
@@ -339,32 +342,32 @@
     </xf>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -676,27 +679,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.83203125" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="3" max="3" width="101.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" customWidth="1"/>
-    <col min="10" max="10" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
+    <col min="3" max="3" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="6.75" customHeight="1"/>
-    <row r="2" spans="2:10" ht="18">
+    <row r="1" spans="2:10" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
@@ -709,7 +711,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -738,7 +740,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:10" hidden="1">
+    <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -759,7 +761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -786,10 +788,10 @@
         <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>5</v>
       </c>
@@ -816,10 +818,10 @@
         <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" hidden="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -840,7 +842,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>19</v>
       </c>
@@ -867,10 +869,10 @@
         <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>21</v>
       </c>
@@ -897,10 +899,10 @@
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" hidden="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
@@ -921,7 +923,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>22</v>
       </c>
@@ -948,7 +950,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:10" hidden="1">
+    <row r="12" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>11</v>
       </c>
@@ -969,7 +971,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="13" spans="2:10" hidden="1">
+    <row r="13" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>13</v>
       </c>
@@ -990,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>24</v>
       </c>
@@ -1017,7 +1019,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="2:10" hidden="1">
+    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>15</v>
       </c>
@@ -1038,7 +1040,7 @@
         <v>0.61904761904761907</v>
       </c>
     </row>
-    <row r="16" spans="2:10" hidden="1">
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>16</v>
       </c>
@@ -1059,7 +1061,7 @@
         <v>1.625</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>25</v>
       </c>
@@ -1083,13 +1085,10 @@
         <v>1</v>
       </c>
       <c r="I17">
-        <v>90</v>
-      </c>
-      <c r="J17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>26</v>
       </c>
@@ -1116,7 +1115,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>27</v>
       </c>
@@ -1143,7 +1142,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>29</v>
       </c>
@@ -1170,7 +1169,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:10">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>33</v>
       </c>
@@ -1194,10 +1193,13 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
+        <v>80</v>
+      </c>
+      <c r="J21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>35</v>
       </c>
@@ -1224,10 +1226,10 @@
         <v>50</v>
       </c>
       <c r="J22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" hidden="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>23</v>
       </c>
@@ -1248,7 +1250,7 @@
         <v>1.6666666666666667</v>
       </c>
     </row>
-    <row r="24" spans="2:10">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>17</v>
       </c>
@@ -1275,7 +1277,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="2:10">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>18</v>
       </c>
@@ -1302,7 +1304,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="2:10">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>20</v>
       </c>
@@ -1326,10 +1328,10 @@
         <v>2</v>
       </c>
       <c r="J26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>30</v>
       </c>
@@ -1353,13 +1355,13 @@
         <v>2</v>
       </c>
       <c r="I27">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="J27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>31</v>
       </c>
@@ -1383,13 +1385,13 @@
         <v>2</v>
       </c>
       <c r="I28">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="J28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>39</v>
       </c>
@@ -1413,10 +1415,10 @@
         <v>2</v>
       </c>
       <c r="J29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>41</v>
       </c>
@@ -1440,10 +1442,10 @@
         <v>2</v>
       </c>
       <c r="J30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>43</v>
       </c>
@@ -1467,10 +1469,10 @@
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>7</v>
       </c>
@@ -1494,13 +1496,13 @@
         <v>3</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="J32" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>37</v>
       </c>
@@ -1527,7 +1529,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:10" hidden="1">
+    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>34</v>
       </c>
@@ -1548,7 +1550,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="35" spans="2:10">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>38</v>
       </c>
@@ -1575,7 +1577,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="2:10">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>40</v>
       </c>
@@ -1602,7 +1604,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:10">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>42</v>
       </c>
@@ -1626,10 +1628,10 @@
         <v>3</v>
       </c>
       <c r="J37" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
         <v>8</v>
       </c>
@@ -1652,11 +1654,14 @@
       <c r="H38">
         <v>4</v>
       </c>
+      <c r="I38">
+        <v>90</v>
+      </c>
       <c r="J38" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="6">
         <v>10</v>
       </c>
@@ -1680,10 +1685,10 @@
         <v>4</v>
       </c>
       <c r="J39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="6">
         <v>14</v>
       </c>
@@ -1707,10 +1712,10 @@
         <v>4</v>
       </c>
       <c r="J40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="6">
         <v>28</v>
       </c>
@@ -1733,11 +1738,14 @@
       <c r="H41">
         <v>4</v>
       </c>
+      <c r="I41">
+        <v>50</v>
+      </c>
       <c r="J41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="6">
         <v>32</v>
       </c>
@@ -1760,11 +1768,11 @@
       <c r="H42">
         <v>4</v>
       </c>
-      <c r="J42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" hidden="1">
+      <c r="I42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>44</v>
       </c>
@@ -1785,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:10">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="6">
         <v>45</v>
       </c>
@@ -1809,10 +1817,10 @@
         <v>4</v>
       </c>
       <c r="J44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" hidden="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>46</v>
       </c>
@@ -1833,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="6">
         <v>47</v>
       </c>
@@ -1860,7 +1868,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="2:10" hidden="1">
+    <row r="47" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>48</v>
       </c>
@@ -1881,7 +1889,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="50" spans="3:3">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizacao das tags concluidas no BackLog
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Product BackLog.xlsx
+++ b/Trunk/Doc/Product BackLog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto Final\fusioness\Trunk\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -408,7 +408,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:J49" totalsRowShown="0">
-  <autoFilter ref="B3:J49"/>
+  <autoFilter ref="B3:J49">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Mobile"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="9">
     <tableColumn id="1" name="#"/>
     <tableColumn id="2" name="User History"/>
@@ -691,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,7 +756,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>4</v>
       </c>
@@ -777,7 +783,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>5</v>
       </c>
@@ -827,8 +833,11 @@
       <c r="H6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>19</v>
       </c>
@@ -855,7 +864,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>21</v>
       </c>
@@ -904,7 +913,7 @@
         <v>2.6666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>22</v>
       </c>
@@ -951,8 +960,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>24</v>
       </c>
@@ -1000,6 +1012,9 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>0.61904761904761907</v>
       </c>
+      <c r="I13">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -1024,8 +1039,11 @@
       <c r="H14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>25</v>
       </c>
@@ -1055,7 +1073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>26</v>
       </c>
@@ -1083,7 +1101,7 @@
       </c>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <v>27</v>
       </c>
@@ -1111,7 +1129,7 @@
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>29</v>
       </c>
@@ -1138,7 +1156,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>33</v>
       </c>
@@ -1165,7 +1183,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>35</v>
       </c>
@@ -1212,8 +1230,11 @@
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1.6666666666666667</v>
       </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
         <v>17</v>
       </c>
@@ -1241,7 +1262,7 @@
       </c>
       <c r="J22" s="4"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>18</v>
       </c>
@@ -1269,7 +1290,7 @@
       </c>
       <c r="J23" s="4"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>20</v>
       </c>
@@ -1297,7 +1318,7 @@
       </c>
       <c r="J24" s="4"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>30</v>
       </c>
@@ -1325,7 +1346,7 @@
       </c>
       <c r="J25" s="4"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>31</v>
       </c>
@@ -1353,7 +1374,7 @@
       </c>
       <c r="J26" s="4"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>39</v>
       </c>
@@ -1381,7 +1402,7 @@
       </c>
       <c r="J27" s="4"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>41</v>
       </c>
@@ -1409,7 +1430,7 @@
       </c>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="2:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>43</v>
       </c>
@@ -1439,7 +1460,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>7</v>
       </c>
@@ -1574,13 +1595,13 @@
         <v>3</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J34" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="6">
         <v>8</v>
       </c>
@@ -1608,7 +1629,7 @@
       </c>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
         <v>10</v>
       </c>
@@ -1638,7 +1659,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="6">
         <v>14</v>
       </c>
@@ -1668,7 +1689,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
         <v>28</v>
       </c>
@@ -1696,7 +1717,7 @@
       </c>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="6">
         <v>32</v>
       </c>
@@ -1745,7 +1766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6">
         <v>45</v>
       </c>
@@ -1796,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" s="6">
         <v>47</v>
       </c>
@@ -1846,7 +1867,9 @@
       <c r="H44" s="8">
         <v>5</v>
       </c>
-      <c r="I44" s="8"/>
+      <c r="I44" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="8">
@@ -1871,7 +1894,9 @@
       <c r="H45" s="8">
         <v>5</v>
       </c>
-      <c r="I45" s="8"/>
+      <c r="I45" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="8">
@@ -1896,7 +1921,9 @@
       <c r="H46" s="8">
         <v>5</v>
       </c>
-      <c r="I46" s="8"/>
+      <c r="I46" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="8">
@@ -1921,7 +1948,9 @@
       <c r="H47" s="8">
         <v>5</v>
       </c>
-      <c r="I47" s="8"/>
+      <c r="I47" s="8">
+        <v>100</v>
+      </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="8">
@@ -1946,7 +1975,9 @@
       <c r="H48" s="8">
         <v>6</v>
       </c>
-      <c r="I48" s="8"/>
+      <c r="I48" s="8">
+        <v>80</v>
+      </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="8">
@@ -1970,7 +2001,9 @@
       <c r="H49" s="8">
         <v>5</v>
       </c>
-      <c r="I49" s="8"/>
+      <c r="I49" s="8">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Corrigido: Quando se respondia a algum convite de evento, este evendo sumia. Corrigido: Listava todos os eventos, agora apenas os que não aconteceram ainda.
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Product BackLog.xlsx
+++ b/Trunk/Doc/Product BackLog.xlsx
@@ -5,14 +5,15 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\fusioness\Trunk\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudo\Bitbucket\fusioness\Trunk\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="14775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="14775" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
   <si>
     <t>#</t>
   </si>
@@ -186,6 +187,21 @@
   </si>
   <si>
     <t>Como usuário gostaria de fazer Login.</t>
+  </si>
+  <si>
+    <t>quando responde um convite de evento, este convite some da lista de "Convites de Eventos"</t>
+  </si>
+  <si>
+    <t>não tem busca de evento</t>
+  </si>
+  <si>
+    <t>na busca de usuários (em contatos) refazer a consulta com AJAX</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -225,7 +241,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +251,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,7 +308,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -299,6 +321,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -307,32 +333,32 @@
     </xf>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -371,13 +397,10 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:J49" totalsRowShown="0">
-  <autoFilter ref="B3:J49">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="0"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B3:J49"/>
+  <sortState ref="B4:J49">
+    <sortCondition descending="1" ref="D3:D49"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="#" dataDxfId="2"/>
     <tableColumn id="2" name="User History" dataDxfId="1"/>
@@ -660,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C42"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,17 +704,17 @@
       <c r="C1"/>
     </row>
     <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -722,7 +745,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -749,7 +772,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -776,107 +799,109 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>8</v>
       </c>
       <c r="G6">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.6666666666666665</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G7">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I7">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G8">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.6666666666666665</v>
+        <v>1.5</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8">
-        <v>100</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G9">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>6</v>
@@ -888,259 +913,262 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.6</v>
+      </c>
+      <c r="H10" s="2">
         <v>2</v>
       </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.5</v>
-      </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="2">
+        <v>100</v>
+      </c>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>5</v>
-      </c>
-      <c r="I11">
-        <v>100</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>100</v>
+      </c>
+      <c r="J11" s="2"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>5</v>
-      </c>
-      <c r="F12">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>6</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>8</v>
+      </c>
+      <c r="G12" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2">
+        <v>100</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2</v>
+      </c>
+      <c r="I13" s="2">
+        <v>100</v>
+      </c>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>2.5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2">
+        <v>100</v>
+      </c>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>8</v>
+      </c>
+      <c r="G15" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>100</v>
+      </c>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2">
+        <v>100</v>
+      </c>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>20</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.6</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
+        <v>100</v>
+      </c>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
         <v>21</v>
       </c>
-      <c r="F13">
+      <c r="C18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G13">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>0.61904761904761907</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-      <c r="I13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <v>11</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>8</v>
-      </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-      <c r="G14">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.625</v>
-      </c>
-      <c r="H14">
-        <v>5</v>
-      </c>
-      <c r="I14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>12</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
-        <v>8</v>
-      </c>
-      <c r="G15" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H15" s="2">
-        <v>2</v>
-      </c>
-      <c r="I15" s="2">
-        <v>100</v>
-      </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>13</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="2">
-        <v>3</v>
-      </c>
-      <c r="F16" s="2">
-        <v>3</v>
-      </c>
-      <c r="G16" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="2">
-        <v>2</v>
-      </c>
-      <c r="I16" s="2">
-        <v>100</v>
-      </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>14</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="2">
-        <v>3</v>
-      </c>
-      <c r="F17" s="2">
-        <v>8</v>
-      </c>
-      <c r="G17" s="2">
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="H17" s="2">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2">
-        <v>100</v>
-      </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2">
+        <v>100</v>
+      </c>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="2">
-        <v>3</v>
-      </c>
-      <c r="F18" s="2">
-        <v>3</v>
-      </c>
-      <c r="G18" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-      <c r="H18" s="2">
-        <v>2</v>
-      </c>
-      <c r="I18" s="2">
-        <v>100</v>
-      </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <v>16</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
@@ -1163,43 +1191,43 @@
       </c>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G20" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.6666666666666665</v>
+        <v>1.5</v>
       </c>
       <c r="H20" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I20" s="2">
         <v>100</v>
       </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="2">
         <v>3</v>
@@ -1212,19 +1240,19 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="H21" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I21" s="2">
         <v>100</v>
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>9</v>
@@ -1233,54 +1261,54 @@
         <v>3</v>
       </c>
       <c r="F22" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G22" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6666666666666667</v>
+        <v>1</v>
       </c>
       <c r="H22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I22" s="2">
         <v>100</v>
       </c>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <v>20</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F23" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G23" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="H23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="2">
         <v>100</v>
       </c>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>21</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>9</v>
@@ -1289,26 +1317,26 @@
         <v>3</v>
       </c>
       <c r="F24" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G24" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.6666666666666665</v>
+        <v>1</v>
       </c>
       <c r="H24" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I24" s="2">
         <v>100</v>
       </c>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>9</v>
@@ -1317,11 +1345,11 @@
         <v>2</v>
       </c>
       <c r="F25" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G25" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="H25" s="2">
         <v>1</v>
@@ -1329,83 +1357,83 @@
       <c r="I25" s="2">
         <v>100</v>
       </c>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="2">
+        <v>3</v>
+      </c>
+      <c r="F26" s="2">
+        <v>8</v>
+      </c>
+      <c r="G26" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>100</v>
+      </c>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="2">
+        <v>8</v>
+      </c>
+      <c r="G27" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.6</v>
+      </c>
+      <c r="H27" s="2">
         <v>2</v>
       </c>
-      <c r="F26" s="2">
-        <v>3</v>
-      </c>
-      <c r="G26" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.5</v>
-      </c>
-      <c r="H26" s="2">
-        <v>4</v>
-      </c>
-      <c r="I26" s="2">
-        <v>100</v>
-      </c>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>24</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="2">
-        <v>3</v>
-      </c>
-      <c r="F27" s="2">
-        <v>5</v>
-      </c>
-      <c r="G27" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6666666666666667</v>
-      </c>
-      <c r="H27" s="2">
-        <v>1</v>
-      </c>
       <c r="I27" s="2">
         <v>100</v>
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E28" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F28" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G28" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="H28" s="2">
         <v>2</v>
@@ -1415,282 +1443,275 @@
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F29" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G29" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>0.66666666666666663</v>
+        <v>1.6</v>
       </c>
       <c r="H29" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I29" s="2">
-        <v>100</v>
-      </c>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
+        <v>38</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>6</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>40</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2">
+        <v>5</v>
+      </c>
+      <c r="F31" s="2">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>4</v>
+      </c>
+      <c r="I31" s="2">
+        <v>100</v>
+      </c>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <v>3</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="2">
-        <v>3</v>
-      </c>
-      <c r="F30" s="2">
-        <v>3</v>
-      </c>
-      <c r="G30" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-      <c r="H30" s="2">
-        <v>4</v>
-      </c>
-      <c r="I30" s="2">
-        <v>100</v>
-      </c>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
+      <c r="D32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="6">
+        <v>3</v>
+      </c>
+      <c r="F32" s="6">
+        <v>8</v>
+      </c>
+      <c r="G32" s="6">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="H32" s="6">
+        <v>5</v>
+      </c>
+      <c r="I32" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>5</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+      <c r="I33">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>8</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="I34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>10</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>21</v>
+      </c>
+      <c r="F35">
+        <v>13</v>
+      </c>
+      <c r="G35">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>0.61904761904761907</v>
+      </c>
+      <c r="H35">
+        <v>5</v>
+      </c>
+      <c r="I35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>11</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+      <c r="F36">
+        <v>13</v>
+      </c>
+      <c r="G36">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.625</v>
+      </c>
+      <c r="H36">
+        <v>5</v>
+      </c>
+      <c r="I36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>18</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="2">
+        <v>3</v>
+      </c>
+      <c r="F37" s="2">
+        <v>5</v>
+      </c>
+      <c r="G37" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="H37" s="2">
+        <v>5</v>
+      </c>
+      <c r="I37" s="2">
+        <v>100</v>
+      </c>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>28</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="2">
-        <v>5</v>
-      </c>
-      <c r="F31" s="2">
-        <v>8</v>
-      </c>
-      <c r="G31" s="2">
+      <c r="D38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="2">
+        <v>5</v>
+      </c>
+      <c r="F38" s="2">
+        <v>8</v>
+      </c>
+      <c r="G38" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
         <v>1.6</v>
       </c>
-      <c r="H31" s="2">
-        <v>3</v>
-      </c>
-      <c r="I31" s="2">
-        <v>100</v>
-      </c>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
-        <v>29</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="2">
-        <v>5</v>
-      </c>
-      <c r="F32" s="2">
-        <v>8</v>
-      </c>
-      <c r="G32" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H32" s="2">
-        <v>3</v>
-      </c>
-      <c r="I32" s="2">
-        <v>100</v>
-      </c>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
-        <v>30</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="2">
-        <v>5</v>
-      </c>
-      <c r="F33" s="2">
-        <v>8</v>
-      </c>
-      <c r="G33" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H33" s="2">
-        <v>3</v>
-      </c>
-      <c r="I33" s="2">
-        <v>100</v>
-      </c>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
-        <v>31</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="2">
-        <v>5</v>
-      </c>
-      <c r="F34" s="2">
-        <v>8</v>
-      </c>
-      <c r="G34" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H34" s="2">
-        <v>3</v>
-      </c>
-      <c r="I34" s="2">
-        <v>100</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
-        <v>32</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="2">
-        <v>2</v>
-      </c>
-      <c r="F35" s="2">
-        <v>8</v>
-      </c>
-      <c r="G35" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>4</v>
-      </c>
-      <c r="H35" s="2">
-        <v>1</v>
-      </c>
-      <c r="I35" s="2">
-        <v>100</v>
-      </c>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
-        <v>33</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="2">
-        <v>3</v>
-      </c>
-      <c r="F36" s="2">
-        <v>8</v>
-      </c>
-      <c r="G36" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>2.6666666666666665</v>
-      </c>
-      <c r="H36" s="2">
-        <v>1</v>
-      </c>
-      <c r="I36" s="2">
-        <v>100</v>
-      </c>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="2">
-        <v>34</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="2">
-        <v>5</v>
-      </c>
-      <c r="F37" s="2">
-        <v>8</v>
-      </c>
-      <c r="G37" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
-      <c r="H37" s="2">
-        <v>2</v>
-      </c>
-      <c r="I37" s="2">
-        <v>100</v>
-      </c>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="2">
-        <v>35</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="2">
-        <v>5</v>
-      </c>
-      <c r="F38" s="2">
-        <v>8</v>
-      </c>
-      <c r="G38" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1.6</v>
-      </c>
       <c r="H38" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I38" s="2">
         <v>100</v>
@@ -1699,13 +1720,13 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" s="2">
         <v>5</v>
@@ -1718,19 +1739,19 @@
         <v>1.6</v>
       </c>
       <c r="H39" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I39" s="2">
-        <v>0</v>
-      </c>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>8</v>
@@ -1739,14 +1760,14 @@
         <v>5</v>
       </c>
       <c r="F40" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G40" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="H40" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I40" s="2">
         <v>100</v>
@@ -1755,47 +1776,49 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="2">
         <v>5</v>
       </c>
       <c r="F41" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G41" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
+        <v>1.6</v>
       </c>
       <c r="H41" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I41" s="2">
-        <v>0</v>
-      </c>
-      <c r="J41" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F42" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G42" s="2">
         <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
@@ -1805,39 +1828,39 @@
         <v>6</v>
       </c>
       <c r="I42" s="2">
+        <v>100</v>
+      </c>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>39</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="2">
+        <v>8</v>
+      </c>
+      <c r="F43" s="2">
+        <v>8</v>
+      </c>
+      <c r="G43" s="2">
+        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
+        <v>1</v>
+      </c>
+      <c r="H43" s="2">
+        <v>6</v>
+      </c>
+      <c r="I43" s="2">
         <v>0</v>
       </c>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="2">
-        <v>40</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="2">
-        <v>5</v>
-      </c>
-      <c r="F43" s="2">
-        <v>5</v>
-      </c>
-      <c r="G43" s="2">
-        <f>Table2[[#This Row],[Business Value]]/Table2[[#This Row],[Story Point]]</f>
-        <v>1</v>
-      </c>
-      <c r="H43" s="2">
-        <v>4</v>
-      </c>
-      <c r="I43" s="2">
-        <v>100</v>
-      </c>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>41</v>
       </c>
@@ -1865,7 +1888,7 @@
       </c>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>42</v>
       </c>
@@ -1893,7 +1916,7 @@
       </c>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>43</v>
       </c>
@@ -1921,7 +1944,7 @@
       </c>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>44</v>
       </c>
@@ -1949,7 +1972,7 @@
       </c>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>45</v>
       </c>
@@ -1977,7 +2000,7 @@
       </c>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <v>46</v>
       </c>
@@ -2022,4 +2045,46 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="85.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Atualizacao da documentacao da Sprint #6
</commit_message>
<xml_diff>
--- a/Trunk/Doc/Product BackLog.xlsx
+++ b/Trunk/Doc/Product BackLog.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudo\Bitbucket\fusioness\Trunk\Doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="14775" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -202,6 +197,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Não Informado</t>
   </si>
 </sst>
 </file>
@@ -397,7 +395,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B3:J49" totalsRowShown="0">
-  <autoFilter ref="B3:J49"/>
+  <autoFilter ref="B3:J49">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="6"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="B4:J49">
     <sortCondition descending="1" ref="D3:D49"/>
   </sortState>
@@ -673,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -683,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -772,7 +776,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -799,7 +803,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -853,7 +857,9 @@
       <c r="I7">
         <v>0</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
@@ -881,7 +887,9 @@
       <c r="I8">
         <v>0</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
@@ -909,9 +917,11 @@
       <c r="I9">
         <v>0</v>
       </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>12</v>
       </c>
@@ -939,7 +949,7 @@
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>13</v>
       </c>
@@ -967,7 +977,7 @@
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>14</v>
       </c>
@@ -995,7 +1005,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>15</v>
       </c>
@@ -1023,7 +1033,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>16</v>
       </c>
@@ -1051,7 +1061,7 @@
       </c>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>17</v>
       </c>
@@ -1079,7 +1089,7 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>19</v>
       </c>
@@ -1107,7 +1117,7 @@
       </c>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>20</v>
       </c>
@@ -1135,7 +1145,7 @@
       </c>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>21</v>
       </c>
@@ -1163,7 +1173,7 @@
       </c>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>22</v>
       </c>
@@ -1191,7 +1201,7 @@
       </c>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>23</v>
       </c>
@@ -1219,7 +1229,7 @@
       </c>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>24</v>
       </c>
@@ -1247,7 +1257,7 @@
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>25</v>
       </c>
@@ -1275,7 +1285,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>26</v>
       </c>
@@ -1303,7 +1313,7 @@
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>27</v>
       </c>
@@ -1331,7 +1341,7 @@
       </c>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>32</v>
       </c>
@@ -1359,7 +1369,7 @@
       </c>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>33</v>
       </c>
@@ -1387,7 +1397,7 @@
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>34</v>
       </c>
@@ -1415,7 +1425,7 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>35</v>
       </c>
@@ -1469,7 +1479,9 @@
       <c r="I29" s="2">
         <v>0</v>
       </c>
-      <c r="J29" s="3"/>
+      <c r="J29" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
@@ -1497,9 +1509,11 @@
       <c r="I30" s="2">
         <v>0</v>
       </c>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>40</v>
       </c>
@@ -1527,7 +1541,7 @@
       </c>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
         <v>3</v>
       </c>
@@ -1554,7 +1568,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>5</v>
       </c>
@@ -1581,7 +1595,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>8</v>
       </c>
@@ -1608,7 +1622,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>10</v>
       </c>
@@ -1635,7 +1649,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>11</v>
       </c>
@@ -1662,7 +1676,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>18</v>
       </c>
@@ -1690,7 +1704,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>28</v>
       </c>
@@ -1718,7 +1732,7 @@
       </c>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>29</v>
       </c>
@@ -1746,7 +1760,7 @@
       </c>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>30</v>
       </c>
@@ -1774,7 +1788,7 @@
       </c>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>31</v>
       </c>
@@ -1856,11 +1870,11 @@
         <v>6</v>
       </c>
       <c r="I43" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>41</v>
       </c>
@@ -1888,7 +1902,7 @@
       </c>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>42</v>
       </c>
@@ -1916,7 +1930,7 @@
       </c>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>43</v>
       </c>
@@ -1944,7 +1958,7 @@
       </c>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>44</v>
       </c>
@@ -2000,7 +2014,7 @@
       </c>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <v>46</v>
       </c>
@@ -2051,7 +2065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>

</xml_diff>